<commit_message>
ablation and resection comparison
</commit_message>
<xml_diff>
--- a/output/supplemental_figures/validation_test_results.xlsx
+++ b/output/supplemental_figures/validation_test_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="55">
   <si>
     <t>Row</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -208,14 +208,110 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,194 +337,194 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="49" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="49" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="49" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="49" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="49" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="49" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>